<commit_message>
basic fields and few-shots prompting
</commit_message>
<xml_diff>
--- a/SOV_docs/LaBarre/LaBarre1_SOV.xlsx
+++ b/SOV_docs/LaBarre/LaBarre1_SOV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JakeJeong\Desktop\Quote\Pending\12.01 - Albrook Condominium Association\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadavkolevesoh/Documents/work/SOVParser/SOV_docs/LaBarre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C7972E-BE9D-49AB-940F-0D14CA793903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49011A1E-29E6-A94A-8FCB-E759F405D355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13575" yWindow="435" windowWidth="19350" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
   <si>
     <t>STATEMENT OF VALUES FOR:</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>Livable Square Footage</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -484,6 +487,19 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -492,22 +508,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -822,63 +822,63 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="5" max="5" width="29.5" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" customWidth="1"/>
+    <col min="8" max="8" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7"/>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="35"/>
-    </row>
-    <row r="2" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D1" s="40"/>
+    </row>
+    <row r="2" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="36">
+      <c r="C2" s="41">
         <v>45992</v>
       </c>
-      <c r="D2" s="37"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="42"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B4" s="33" t="s">
         <v>59</v>
       </c>
@@ -886,33 +886,38 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+    <row r="5" spans="1:17" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A5" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="39" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+    </row>
+    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="30">
         <v>1</v>
       </c>
@@ -936,7 +941,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="30">
         <v>2</v>
       </c>
@@ -960,7 +965,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="30">
         <v>3</v>
       </c>
@@ -983,8 +988,11 @@
       <c r="H8" s="22">
         <v>1800</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="30">
         <v>4</v>
       </c>
@@ -1007,8 +1015,11 @@
       <c r="H9" s="22">
         <v>1500</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="30">
         <v>5</v>
       </c>
@@ -1031,8 +1042,11 @@
       <c r="H10" s="22">
         <v>1500</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="30">
         <v>6</v>
       </c>
@@ -1055,8 +1069,11 @@
       <c r="H11" s="22">
         <v>1500</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="30">
         <v>7</v>
       </c>
@@ -1079,8 +1096,11 @@
       <c r="H12" s="22">
         <v>1500</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="30">
         <v>8</v>
       </c>
@@ -1103,8 +1123,11 @@
       <c r="H13" s="22">
         <v>1200</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="30">
         <v>9</v>
       </c>
@@ -1127,18 +1150,24 @@
       <c r="H14" s="22">
         <v>1200</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="Q15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
         <v>10</v>
       </c>
@@ -1149,7 +1178,7 @@
         <f>SUM(E6:E14)</f>
         <v>10053858</v>
       </c>
-      <c r="F16" s="39">
+      <c r="F16" s="36">
         <f>SUM(F6:F14)</f>
         <v>44</v>
       </c>
@@ -1162,10 +1191,10 @@
         <v>13200</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>11</v>
       </c>
@@ -1179,7 +1208,7 @@
       <c r="E18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F18" s="35">
         <v>1</v>
       </c>
       <c r="G18" s="18" t="s">
@@ -1190,7 +1219,7 @@
         <v>69469</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>16</v>
       </c>
@@ -1211,7 +1240,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>20</v>
       </c>
@@ -1232,7 +1261,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>23</v>
       </c>
@@ -1253,7 +1282,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>27</v>
       </c>
@@ -1274,7 +1303,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>31</v>
       </c>
@@ -1295,7 +1324,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
         <v>58</v>
       </c>
@@ -1316,7 +1345,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="13"/>
       <c r="C25" s="14"/>
@@ -1331,7 +1360,7 @@
         <v>10188858</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="13"/>
       <c r="C26" s="14"/>
@@ -1345,7 +1374,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="16"/>
       <c r="C27" s="29"/>
@@ -1361,7 +1390,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>39</v>
       </c>
@@ -1424,15 +1453,15 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>41</v>
       </c>
@@ -1452,7 +1481,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>44</v>
       </c>
@@ -1472,7 +1501,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>19</v>
       </c>
@@ -1493,7 +1522,7 @@
       </c>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>52</v>
       </c>
@@ -1507,7 +1536,7 @@
       </c>
       <c r="F4" s="16"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
       <c r="B5" s="16" t="s">
         <v>55</v>
@@ -1517,7 +1546,7 @@
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="16" t="s">
         <v>56</v>
@@ -1527,7 +1556,7 @@
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -1546,28 +1575,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010098C78C132932754C8148AF12D17B3413" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f3e0f26296dc6b8688be0a0b54b5993">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2fdb0ffa457db17e93317e727f8a95b7">
     <xsd:element name="properties">
@@ -1681,10 +1695,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08F7A9FD-5A42-4E85-995F-FF50B830BB28}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8423A50-1AFA-4D8D-A52F-AE356BFB8EC1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1699,17 +1736,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8423A50-1AFA-4D8D-A52F-AE356BFB8EC1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08F7A9FD-5A42-4E85-995F-FF50B830BB28}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>